<commit_message>
[Document, Modified] : MyMusic Thiết kế xử lý
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/MyMusic/MyMucsic.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/MyMusic/MyMucsic.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="132">
   <si>
     <t>DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -117,7 +117,7 @@
     <t>List&lt;Music&gt;</t>
   </si>
   <si>
-    <t>Vét cạn</t>
+    <t>N/A</t>
   </si>
   <si>
     <t>Truyền userId xuống controller và nhận danh sách music  từ controller</t>
@@ -153,7 +153,10 @@
     <t xml:space="preserve"> Thêm music</t>
   </si>
   <si>
-    <t>getMusic()</t>
+    <t>readMusic_Controller()</t>
+  </si>
+  <si>
+    <t>Vét cạn</t>
   </si>
   <si>
     <t>Truyền userId từ view xuống CSDL và nhận danh sách music từ CSDL</t>
@@ -231,6 +234,12 @@
     <t>Định nghỉ hành động mở form</t>
   </si>
   <si>
+    <t>playMusic_Controller()</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nhị phân</t>
+  </si>
+  <si>
     <t>Phát bài hát</t>
   </si>
   <si>
@@ -279,6 +288,9 @@
     <t>Số lượng ký tự tối đa của tên music</t>
   </si>
   <si>
+    <t>pauseMusic_Controller()</t>
+  </si>
+  <si>
     <t>Tạm dừng bài hát</t>
   </si>
   <si>
@@ -318,6 +330,9 @@
     <t>Lưu file bài hát</t>
   </si>
   <si>
+    <t>stopMusic_Controller()</t>
+  </si>
+  <si>
     <t>Ngừng phát</t>
   </si>
   <si>
@@ -339,16 +354,10 @@
     <t>File music</t>
   </si>
   <si>
-    <t>Truyền file music mới xuống controller</t>
+    <t>Truyền file music mới xuống controller và nhận danh sách music đã cập nhật từ Controller</t>
   </si>
   <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU File</t>
-  </si>
-  <si>
-    <t>displayMusic()</t>
-  </si>
-  <si>
-    <t>Hiển thị danh sách music lên màn hình</t>
   </si>
   <si>
     <t>checkFileUpload()</t>
@@ -357,25 +366,40 @@
     <t xml:space="preserve">Kiểm tra file upload </t>
   </si>
   <si>
+    <t>uploadMusic_Controller()</t>
+  </si>
+  <si>
+    <t>Truyền file music mới từ controller xuống CSDL và thêm bài hát vào danh sách, gửi danh sách music đã cập nhật lên view</t>
+  </si>
+  <si>
     <t>File có định dạng : *.mp3</t>
   </si>
   <si>
-    <t>Truyền file music mới từ controller xuống CSDL</t>
+    <t>uploadMusic_DAO()</t>
   </si>
   <si>
     <t>Thêm file music dưới CSDL</t>
   </si>
   <si>
+    <t>deleteMusic()</t>
+  </si>
+  <si>
+    <t>Truyền musicId xuống controller và nhận danh sách music đã cập nhật từ Controller</t>
+  </si>
+  <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU MusicDAO</t>
   </si>
   <si>
-    <t>deleteMusic()</t>
+    <t>deleteMusic_Controller()</t>
   </si>
   <si>
-    <t>Truyền musicId xuống controller</t>
+    <t>Truyền musicId từ controller xuống CSDL và xóa, gửi danh sách music đã cập nhật lên view</t>
   </si>
   <si>
-    <t>Truyền musicId từ controller xuống CSDL</t>
+    <t>deleteMusic_DAO()</t>
+  </si>
+  <si>
+    <t>Xóa music dưới CSDL</t>
   </si>
   <si>
     <t>new MusicDAO()</t>
@@ -383,9 +407,6 @@
   <si>
     <t>Phương thức khởi tạo 
 của class MusicDao</t>
-  </si>
-  <si>
-    <t>Xóa music dưới CSDL</t>
   </si>
   <si>
     <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU int</t>
@@ -404,10 +425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -456,21 +477,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -478,9 +484,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,8 +506,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,9 +531,47 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -533,14 +584,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -554,37 +598,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -594,7 +607,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -609,7 +630,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,7 +642,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,49 +726,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,7 +756,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,31 +786,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,61 +810,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,26 +893,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -916,6 +937,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -954,33 +990,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -992,134 +1013,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1178,7 +1199,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1507,8 +1527,8 @@
   <sheetPr/>
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U6" workbookViewId="0">
-      <selection activeCell="AF14" sqref="AF14"/>
+    <sheetView tabSelected="1" topLeftCell="V14" workbookViewId="0">
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -1523,8 +1543,9 @@
     <col min="12" max="19" width="14.4285714285714" style="1"/>
     <col min="20" max="20" width="17.5714285714286" style="1" customWidth="1"/>
     <col min="21" max="26" width="14.4285714285714" style="1"/>
-    <col min="27" max="27" width="18" style="1" customWidth="1"/>
-    <col min="28" max="30" width="14.4285714285714" style="1"/>
+    <col min="27" max="27" width="22.4285714285714" style="1" customWidth="1"/>
+    <col min="28" max="29" width="14.4285714285714" style="1"/>
+    <col min="30" max="30" width="15.8571428571429" style="1" customWidth="1"/>
     <col min="31" max="31" width="18.8571428571429" style="1" customWidth="1"/>
     <col min="32" max="16384" width="14.4285714285714" style="1"/>
   </cols>
@@ -1799,10 +1820,10 @@
         <v>32</v>
       </c>
       <c r="AD4" s="21" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="AE4" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AF4" s="21"/>
     </row>
@@ -1811,7 +1832,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1820,7 +1841,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>23</v>
@@ -1841,7 +1862,7 @@
         <v>23</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="6"/>
       <c r="R5" s="3"/>
@@ -1849,16 +1870,16 @@
         <v>3</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X5" s="5"/>
       <c r="Y5" s="3"/>
@@ -1866,7 +1887,7 @@
         <v>3</v>
       </c>
       <c r="AA5" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AB5" s="21" t="s">
         <v>31</v>
@@ -1874,9 +1895,11 @@
       <c r="AC5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="AD5" s="21"/>
+      <c r="AD5" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE5" s="21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AF5" s="21"/>
     </row>
@@ -1885,10 +1908,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="3"/>
@@ -1896,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>23</v>
@@ -1911,13 +1934,13 @@
         <v>4</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
@@ -1925,16 +1948,16 @@
         <v>4</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="3"/>
@@ -1942,15 +1965,19 @@
         <v>4</v>
       </c>
       <c r="AA6" s="21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB6" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD6" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE6" s="21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AF6" s="21"/>
     </row>
@@ -1959,7 +1986,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1968,7 +1995,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
@@ -1983,13 +2010,13 @@
         <v>5</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q7" s="6"/>
       <c r="R7" s="3"/>
@@ -1997,16 +2024,16 @@
         <v>5</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="U7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W7" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X7" s="5"/>
       <c r="Y7" s="3"/>
@@ -2014,15 +2041,19 @@
         <v>5</v>
       </c>
       <c r="AA7" s="21" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="AB7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD7" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AE7" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AF7" s="21"/>
     </row>
@@ -2031,13 +2062,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E8" s="3"/>
       <c r="L8" s="3"/>
@@ -2045,13 +2076,13 @@
         <v>6</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="3"/>
@@ -2059,16 +2090,16 @@
         <v>6</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="W8" s="6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="X8" s="5"/>
       <c r="Y8" s="3"/>
@@ -2076,15 +2107,19 @@
         <v>6</v>
       </c>
       <c r="AA8" s="21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AB8" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD8" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE8" s="21" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AF8" s="21"/>
     </row>
@@ -2093,13 +2128,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -2111,13 +2146,13 @@
         <v>7</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="3"/>
@@ -2125,7 +2160,7 @@
         <v>7</v>
       </c>
       <c r="T9" s="17" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="U9" s="17" t="s">
         <v>20</v>
@@ -2134,7 +2169,7 @@
         <v>1000</v>
       </c>
       <c r="W9" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="X9" s="17"/>
       <c r="Y9" s="3"/>
@@ -2142,15 +2177,19 @@
         <v>7</v>
       </c>
       <c r="AA9" s="21" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AB9" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC9" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD9" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AE9" s="21" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AF9" s="21"/>
     </row>
@@ -2159,10 +2198,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
@@ -2189,13 +2228,13 @@
         <v>8</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q10" s="6"/>
       <c r="R10" s="3"/>
@@ -2203,7 +2242,7 @@
         <v>8</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="U10" s="13" t="s">
         <v>20</v>
@@ -2212,7 +2251,7 @@
         <v>5</v>
       </c>
       <c r="W10" s="19" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="X10" s="13"/>
       <c r="Y10" s="3"/>
@@ -2220,15 +2259,19 @@
         <v>8</v>
       </c>
       <c r="AA10" s="21" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="AB10" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC10" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD10" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE10" s="21" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="AF10" s="21"/>
     </row>
@@ -2237,7 +2280,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2259,13 +2302,13 @@
         <v>9</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="Q11" s="18"/>
       <c r="R11" s="3"/>
@@ -2280,27 +2323,31 @@
         <v>9</v>
       </c>
       <c r="AA11" s="21" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="AB11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD11" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AE11" s="21" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="AF11" s="21"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+    <row r="12" s="1" customFormat="1" ht="63.75" spans="1:32">
       <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
@@ -2315,13 +2362,13 @@
         <v>10</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="O12" s="13" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="Q12" s="19"/>
       <c r="R12" s="3"/>
@@ -2336,15 +2383,19 @@
         <v>10</v>
       </c>
       <c r="AA12" s="21" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="AB12" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="21"/>
+        <v>110</v>
+      </c>
+      <c r="AC12" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD12" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE12" s="21" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="AF12" s="21"/>
     </row>
@@ -2355,7 +2406,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -2376,23 +2427,27 @@
       <c r="W13" s="20"/>
       <c r="X13" s="20"/>
       <c r="Y13" s="3"/>
-      <c r="Z13" s="21">
-        <v>11</v>
+      <c r="Z13" s="19">
+        <v>12</v>
       </c>
       <c r="AA13" s="21" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AB13" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21"/>
+        <v>110</v>
+      </c>
+      <c r="AC13" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD13" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE13" s="21" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AF13" s="21"/>
     </row>
-    <row r="14" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+    <row r="14" s="1" customFormat="1" ht="76.5" spans="1:32">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2431,22 +2486,26 @@
       <c r="X14" s="20"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AA14" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB14" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AB14" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21"/>
+      <c r="AC14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD14" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE14" s="21" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="AF14" s="21"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="38.25" spans="1:32">
+    <row r="15" s="1" customFormat="1" ht="25.5" spans="1:32">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2456,13 +2515,13 @@
         <v>1</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>25</v>
@@ -2483,22 +2542,26 @@
       <c r="X15" s="20"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="19">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA15" s="21" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="AB15" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC15" s="22"/>
-      <c r="AD15" s="21"/>
+        <v>110</v>
+      </c>
+      <c r="AC15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD15" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE15" s="21" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="AF15" s="21"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:32">
+    <row r="16" s="1" customFormat="1" ht="51" spans="1:32">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2519,29 +2582,33 @@
       <c r="X16" s="20"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="19">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AA16" s="21" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="AB16" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC16" s="22"/>
-      <c r="AD16" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD16" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE16" s="21" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="AF16" s="21"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="25.5" spans="1:32">
+    <row r="17" s="1" customFormat="1" ht="63.75" spans="1:32">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -2563,22 +2630,26 @@
       <c r="X17" s="20"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="19">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AA17" s="21" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="AB17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC17" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD17" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AE17" s="21" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="AF17" s="21"/>
     </row>
-    <row r="18" s="1" customFormat="1" ht="25.5" spans="1:32">
+    <row r="18" s="1" customFormat="1" ht="24" customHeight="1" spans="1:32">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2617,22 +2688,26 @@
       <c r="X18" s="20"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="19">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA18" s="21" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="AB18" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC18" s="21"/>
-      <c r="AD18" s="21"/>
+        <v>63</v>
+      </c>
+      <c r="AC18" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD18" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="AE18" s="21" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="AF18" s="21"/>
     </row>
-    <row r="19" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
+    <row r="19" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2642,17 +2717,17 @@
         <v>1</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="20"/>
@@ -2668,21 +2743,6 @@
       <c r="W19" s="20"/>
       <c r="X19" s="20"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="19">
-        <v>17</v>
-      </c>
-      <c r="AA19" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="AB19" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC19" s="21"/>
-      <c r="AD19" s="21"/>
-      <c r="AE19" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF19" s="21"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A20" s="3"/>
@@ -2710,13 +2770,13 @@
       <c r="W20" s="20"/>
       <c r="X20" s="20"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24"/>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="24"/>
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="23"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="27" customHeight="1" spans="1:32">
       <c r="A21" s="3"/>
@@ -2725,7 +2785,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2746,13 +2806,13 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="25"/>
-      <c r="AD21" s="24"/>
-      <c r="AE21" s="24"/>
-      <c r="AF21" s="24"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="24"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="23"/>
+      <c r="AF21" s="23"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="27" customHeight="1" spans="1:25">
       <c r="A22" s="3"/>
@@ -2803,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>20</v>
@@ -2813,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="20"/>
@@ -2864,7 +2924,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -2935,10 +2995,10 @@
         <v>1</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5" t="s">

</xml_diff>